<commit_message>
Update input with changes (c2c).xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/for paper/input with changes (c2c).xlsx
+++ b/migforecasting/clustering/for paper/input with changes (c2c).xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,60 +767,60 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>1005.041577808463</v>
+        <v>3585.794729443383</v>
       </c>
       <c r="C7" t="n">
         <v>20815.4167831292</v>
       </c>
       <c r="D7" t="n">
-        <v>2244.722876564279</v>
+        <v>4985.602237377395</v>
       </c>
       <c r="E7" t="n">
-        <v>97.90470282409201</v>
+        <v>474.8378086968473</v>
       </c>
       <c r="F7" t="n">
-        <v>83942.99632047053</v>
+        <v>737465.7897395631</v>
       </c>
       <c r="G7" t="n">
-        <v>35.8</v>
+        <v>30.8316326530612</v>
       </c>
       <c r="H7" t="n">
-        <v>15.10365756373615</v>
+        <v>62.73826988013489</v>
       </c>
       <c r="I7" t="n">
-        <v>2.457371038578607</v>
+        <v>39.31793661725785</v>
       </c>
       <c r="J7" t="n">
-        <v>92.93787243569393</v>
+        <v>1231.999999999999</v>
       </c>
       <c r="K7" t="n">
-        <v>35561.25821905064</v>
+        <v>52214.87172571371</v>
       </c>
       <c r="L7" t="n">
-        <v>1524.614084681972</v>
+        <v>10989.33540619813</v>
       </c>
       <c r="M7" t="n">
-        <v>1134350.952355311</v>
+        <v>4717355.206267274</v>
       </c>
       <c r="N7" t="n">
-        <v>10.22528063837951</v>
+        <v>35.75225116085909</v>
       </c>
       <c r="O7" t="n">
-        <v>289.7844042574963</v>
+        <v>1599.139320430128</v>
       </c>
       <c r="P7" t="n">
-        <v>1130904.823893648</v>
+        <v>5013077.512856801</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>5648.558240191881</v>
+        <v>3343.769507917894</v>
       </c>
       <c r="C8" t="n">
         <v>20815.4167831292</v>
@@ -829,13 +829,13 @@
         <v>19721.96170086985</v>
       </c>
       <c r="E8" t="n">
-        <v>34.26664598843221</v>
+        <v>881.0076688693483</v>
       </c>
       <c r="F8" t="n">
-        <v>388747.3300403743</v>
+        <v>690881.1824932072</v>
       </c>
       <c r="G8" t="n">
-        <v>30.8316326530612</v>
+        <v>32.45</v>
       </c>
       <c r="H8" t="n">
         <v>125.6772308691166</v>
@@ -844,425 +844,1175 @@
         <v>77.80585983126005</v>
       </c>
       <c r="J8" t="n">
-        <v>231.3171124750813</v>
+        <v>657.7753259148542</v>
       </c>
       <c r="K8" t="n">
-        <v>314708.9999999999</v>
+        <v>14779.51264709787</v>
       </c>
       <c r="L8" t="n">
-        <v>23252.7844053831</v>
+        <v>39193.22582760982</v>
       </c>
       <c r="M8" t="n">
-        <v>4717355.206267274</v>
+        <v>3164647.335590403</v>
       </c>
       <c r="N8" t="n">
-        <v>35.75225116085909</v>
+        <v>40.99999999999988</v>
       </c>
       <c r="O8" t="n">
         <v>1599.139320430128</v>
       </c>
       <c r="P8" t="n">
-        <v>5013077.512856801</v>
+        <v>765252.0536330917</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="n">
-        <v>2404.96641179009</v>
+        <v>2855.897614000732</v>
       </c>
       <c r="C9" t="n">
         <v>20815.4167831292</v>
       </c>
       <c r="D9" t="n">
-        <v>10460.82771834146</v>
+        <v>6933.370835542808</v>
       </c>
       <c r="E9" t="n">
-        <v>287.5950645457707</v>
+        <v>310.8474314664927</v>
       </c>
       <c r="F9" t="n">
-        <v>494652.2041766169</v>
+        <v>442174.8124846562</v>
       </c>
       <c r="G9" t="n">
         <v>30.8316326530612</v>
       </c>
       <c r="H9" t="n">
-        <v>155.9999999999989</v>
+        <v>63.90008969272994</v>
       </c>
       <c r="I9" t="n">
-        <v>77.80585983126005</v>
+        <v>43.00399317512575</v>
       </c>
       <c r="J9" t="n">
-        <v>657.7753259148542</v>
+        <v>982.8999999999988</v>
       </c>
       <c r="K9" t="n">
-        <v>182951.9999999998</v>
+        <v>25352.01880031726</v>
       </c>
       <c r="L9" t="n">
-        <v>23401.03629808141</v>
+        <v>16214.47648840938</v>
       </c>
       <c r="M9" t="n">
-        <v>4717355.206267274</v>
+        <v>1683505.391251907</v>
       </c>
       <c r="N9" t="n">
         <v>35.75225116085909</v>
       </c>
       <c r="O9" t="n">
-        <v>909.6010466971422</v>
+        <v>798.0570498202485</v>
       </c>
       <c r="P9" t="n">
-        <v>486123.8000606647</v>
+        <v>5013077.512856801</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>20038</v>
+        <v>1599.914095979</v>
       </c>
       <c r="C10" t="n">
-        <v>29031.0083701363</v>
+        <v>20815.4167831292</v>
       </c>
       <c r="D10" t="n">
-        <v>72911.59999999999</v>
+        <v>7805.250292211623</v>
       </c>
       <c r="E10" t="n">
-        <v>2549.999999999998</v>
+        <v>166.4379948009566</v>
       </c>
       <c r="F10" t="n">
-        <v>4713511.93528</v>
+        <v>229335.514217616</v>
       </c>
       <c r="G10" t="n">
-        <v>29.9</v>
+        <v>30.8316326530612</v>
       </c>
       <c r="H10" t="n">
-        <v>195.9999999999987</v>
+        <v>53.44371137937411</v>
       </c>
       <c r="I10" t="n">
-        <v>248.9999999999989</v>
+        <v>11.05816967360375</v>
       </c>
       <c r="J10" t="n">
-        <v>1123.199999999998</v>
+        <v>193.2970737513881</v>
       </c>
       <c r="K10" t="n">
-        <v>1264806.999999999</v>
+        <v>101102.9756497258</v>
       </c>
       <c r="L10" t="n">
-        <v>104307.93</v>
+        <v>16989.97808396383</v>
       </c>
       <c r="M10" t="n">
-        <v>2214641.343439997</v>
+        <v>826863.3503797244</v>
       </c>
       <c r="N10" t="n">
-        <v>34.99999999999991</v>
+        <v>35.75225116085909</v>
       </c>
       <c r="O10" t="n">
-        <v>6308.999999999999</v>
+        <v>466.8748735259664</v>
       </c>
       <c r="P10" t="n">
-        <v>26988496.70547999</v>
+        <v>129328.7338934138</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>8680.999999999998</v>
+        <v>1647.045323328701</v>
       </c>
       <c r="C11" t="n">
         <v>20815.4167831292</v>
       </c>
       <c r="D11" t="n">
-        <v>32935.89999999999</v>
+        <v>5679.851509250544</v>
       </c>
       <c r="E11" t="n">
-        <v>1673.999999999998</v>
+        <v>146.8570542361383</v>
       </c>
       <c r="F11" t="n">
-        <v>1330729.49304</v>
+        <v>317997.2410657947</v>
       </c>
       <c r="G11" t="n">
         <v>30.8316326530612</v>
       </c>
       <c r="H11" t="n">
-        <v>158.9999999999989</v>
+        <v>24.39821606449689</v>
       </c>
       <c r="I11" t="n">
-        <v>184.9999999999992</v>
+        <v>22.11633934720753</v>
       </c>
       <c r="J11" t="n">
-        <v>657.7753259148542</v>
+        <v>175.6000587298496</v>
       </c>
       <c r="K11" t="n">
-        <v>810919.9999999998</v>
+        <v>18464.39264186816</v>
       </c>
       <c r="L11" t="n">
-        <v>182696</v>
+        <v>14618.51135645239</v>
       </c>
       <c r="M11" t="n">
-        <v>5519372.853599999</v>
+        <v>1004420.350031578</v>
       </c>
       <c r="N11" t="n">
-        <v>38.99999999999991</v>
+        <v>15.33792095756929</v>
       </c>
       <c r="O11" t="n">
-        <v>2500</v>
+        <v>507.1227074506192</v>
       </c>
       <c r="P11" t="n">
-        <v>5013077.512856801</v>
+        <v>185968.03543353</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="n">
-        <v>3592.163814220368</v>
+        <v>1005.041577808463</v>
       </c>
       <c r="C12" t="n">
         <v>20815.4167831292</v>
       </c>
       <c r="D12" t="n">
-        <v>19721.96170086985</v>
+        <v>2244.722876564279</v>
       </c>
       <c r="E12" t="n">
-        <v>424.6616484994997</v>
+        <v>97.90470282409201</v>
       </c>
       <c r="F12" t="n">
-        <v>1094086.860592877</v>
+        <v>83942.99632047053</v>
       </c>
       <c r="G12" t="n">
-        <v>30.8316326530612</v>
+        <v>35.8</v>
       </c>
       <c r="H12" t="n">
-        <v>125.6772308691166</v>
+        <v>15.10365756373615</v>
       </c>
       <c r="I12" t="n">
-        <v>77.80585983126005</v>
+        <v>2.457371038578607</v>
       </c>
       <c r="J12" t="n">
-        <v>657.7753259148542</v>
+        <v>92.93787243569393</v>
       </c>
       <c r="K12" t="n">
-        <v>44036.37111627778</v>
+        <v>35561.25821905064</v>
       </c>
       <c r="L12" t="n">
-        <v>11411.26707998794</v>
+        <v>1524.614084681972</v>
       </c>
       <c r="M12" t="n">
-        <v>4717355.206267274</v>
+        <v>1134350.952355311</v>
       </c>
       <c r="N12" t="n">
-        <v>35.75225116085909</v>
+        <v>10.22528063837951</v>
       </c>
       <c r="O12" t="n">
-        <v>856.7038935390278</v>
+        <v>289.7844042574963</v>
       </c>
       <c r="P12" t="n">
-        <v>1248365.758196321</v>
+        <v>1130904.823893648</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="n">
-        <v>21239</v>
+        <v>5648.558240191881</v>
       </c>
       <c r="C13" t="n">
-        <v>29031.0083701363</v>
+        <v>20815.4167831292</v>
       </c>
       <c r="D13" t="n">
-        <v>64664.39999999999</v>
+        <v>19721.96170086985</v>
       </c>
       <c r="E13" t="n">
-        <v>2077</v>
+        <v>34.26664598843221</v>
       </c>
       <c r="F13" t="n">
-        <v>4676977.19118</v>
+        <v>388747.3300403743</v>
       </c>
       <c r="G13" t="n">
-        <v>30.2</v>
+        <v>30.8316326530612</v>
       </c>
       <c r="H13" t="n">
-        <v>300.9999999999981</v>
+        <v>125.6772308691166</v>
       </c>
       <c r="I13" t="n">
-        <v>303.9999999999987</v>
+        <v>77.80585983126005</v>
       </c>
       <c r="J13" t="n">
-        <v>783.7999999999988</v>
+        <v>231.3171124750813</v>
       </c>
       <c r="K13" t="n">
-        <v>202571</v>
+        <v>314708.9999999999</v>
       </c>
       <c r="L13" t="n">
-        <v>87368.90999999997</v>
+        <v>23252.7844053831</v>
       </c>
       <c r="M13" t="n">
-        <v>8408723.879599998</v>
+        <v>4717355.206267274</v>
       </c>
       <c r="N13" t="n">
-        <v>34.9999999999999</v>
+        <v>35.75225116085909</v>
       </c>
       <c r="O13" t="n">
-        <v>4502</v>
+        <v>1599.139320430128</v>
       </c>
       <c r="P13" t="n">
-        <v>25333054.93499543</v>
+        <v>5013077.512856801</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B14" t="n">
-        <v>15029</v>
+        <v>2404.96641179009</v>
       </c>
       <c r="C14" t="n">
-        <v>25869.38778</v>
+        <v>20815.4167831292</v>
       </c>
       <c r="D14" t="n">
-        <v>19151.02604309839</v>
+        <v>10460.82771834146</v>
       </c>
       <c r="E14" t="n">
-        <v>1645.641044300649</v>
+        <v>287.5950645457707</v>
       </c>
       <c r="F14" t="n">
-        <v>1067319.071699882</v>
+        <v>494652.2041766169</v>
       </c>
       <c r="G14" t="n">
-        <v>27.6202945590994</v>
+        <v>30.8316326530612</v>
       </c>
       <c r="H14" t="n">
-        <v>124.9999999999992</v>
+        <v>155.9999999999989</v>
       </c>
       <c r="I14" t="n">
-        <v>194.9999999999991</v>
+        <v>77.80585983126005</v>
       </c>
       <c r="J14" t="n">
-        <v>384.7889277610419</v>
+        <v>657.7753259148542</v>
       </c>
       <c r="K14" t="n">
-        <v>2168.999999999995</v>
+        <v>182951.9999999998</v>
       </c>
       <c r="L14" t="n">
-        <v>24766.25131576219</v>
+        <v>23401.03629808141</v>
       </c>
       <c r="M14" t="n">
-        <v>282905.7514288604</v>
+        <v>4717355.206267274</v>
       </c>
       <c r="N14" t="n">
-        <v>21.09561578308453</v>
+        <v>35.75225116085909</v>
       </c>
       <c r="O14" t="n">
-        <v>3211</v>
+        <v>909.6010466971422</v>
       </c>
       <c r="P14" t="n">
-        <v>9430951.714799995</v>
+        <v>486123.8000606647</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15" t="n">
-        <v>9192</v>
+        <v>20038</v>
       </c>
       <c r="C15" t="n">
-        <v>21205.02672</v>
+        <v>29031.0083701363</v>
       </c>
       <c r="D15" t="n">
-        <v>59994</v>
+        <v>72911.59999999999</v>
       </c>
       <c r="E15" t="n">
-        <v>1042.999999999999</v>
+        <v>2549.999999999998</v>
       </c>
       <c r="F15" t="n">
-        <v>1194600.348719999</v>
+        <v>4713511.93528</v>
       </c>
       <c r="G15" t="n">
-        <v>30.8316326530612</v>
+        <v>29.9</v>
       </c>
       <c r="H15" t="n">
-        <v>140.9999999999991</v>
+        <v>195.9999999999987</v>
       </c>
       <c r="I15" t="n">
-        <v>92.99999999999956</v>
+        <v>248.9999999999989</v>
       </c>
       <c r="J15" t="n">
-        <v>657.7753259148542</v>
+        <v>1123.199999999998</v>
       </c>
       <c r="K15" t="n">
-        <v>39877.13364253051</v>
+        <v>1264806.999999999</v>
       </c>
       <c r="L15" t="n">
-        <v>70633.64091748245</v>
+        <v>104307.93</v>
       </c>
       <c r="M15" t="n">
-        <v>8271274.176000002</v>
+        <v>2214641.343439997</v>
       </c>
       <c r="N15" t="n">
-        <v>36.99999999999991</v>
+        <v>34.99999999999991</v>
       </c>
       <c r="O15" t="n">
-        <v>3090</v>
+        <v>6308.999999999999</v>
       </c>
       <c r="P15" t="n">
-        <v>7029925.234559999</v>
+        <v>26988496.70547999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" t="n">
+        <v>8680.999999999998</v>
+      </c>
+      <c r="C16" t="n">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D16" t="n">
+        <v>32935.89999999999</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1673.999999999998</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1330729.49304</v>
+      </c>
+      <c r="G16" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H16" t="n">
+        <v>158.9999999999989</v>
+      </c>
+      <c r="I16" t="n">
+        <v>184.9999999999992</v>
+      </c>
+      <c r="J16" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K16" t="n">
+        <v>810919.9999999998</v>
+      </c>
+      <c r="L16" t="n">
+        <v>182696</v>
+      </c>
+      <c r="M16" t="n">
+        <v>5519372.853599999</v>
+      </c>
+      <c r="N16" t="n">
+        <v>38.99999999999991</v>
+      </c>
+      <c r="O16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P16" t="n">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1629.211885953139</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2818.518706481017</v>
+      </c>
+      <c r="D17" t="n">
+        <v>347.6177107035295</v>
+      </c>
+      <c r="E17" t="n">
+        <v>415783.7487599998</v>
+      </c>
+      <c r="F17" t="n">
+        <v>67.99398834357636</v>
+      </c>
+      <c r="G17" t="n">
+        <v>37.3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>19.75093681411653</v>
+      </c>
+      <c r="I17" t="n">
+        <v>19.65896830862891</v>
+      </c>
+      <c r="J17" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K17" t="n">
+        <v>101102.9756497258</v>
+      </c>
+      <c r="L17" t="n">
+        <v>9399.12834296009</v>
+      </c>
+      <c r="M17" t="n">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N17" t="n">
+        <v>35.75225116085909</v>
+      </c>
+      <c r="O17" t="n">
+        <v>433.5266682741121</v>
+      </c>
+      <c r="P17" t="n">
+        <v>551974.7321851443</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>3</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2658.455985914151</v>
+      </c>
+      <c r="C18" t="n">
+        <v>7013.102453840388</v>
+      </c>
+      <c r="D18" t="n">
+        <v>260.096939568953</v>
+      </c>
+      <c r="E18" t="n">
+        <v>267414.72804</v>
+      </c>
+      <c r="F18" t="n">
+        <v>21.71341493966039</v>
+      </c>
+      <c r="G18" t="n">
+        <v>32.08</v>
+      </c>
+      <c r="H18" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I18" t="n">
+        <v>77.80585983126005</v>
+      </c>
+      <c r="J18" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K18" t="n">
+        <v>297093.9999999998</v>
+      </c>
+      <c r="L18" t="n">
+        <v>20785.4029544657</v>
+      </c>
+      <c r="M18" t="n">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N18" t="n">
+        <v>39.99999999999989</v>
+      </c>
+      <c r="O18" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P18" t="n">
+        <v>2364731.150852372</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>3</v>
+      </c>
+      <c r="B19" t="n">
+        <v>3425.293793063323</v>
+      </c>
+      <c r="C19" t="n">
+        <v>9827.914734638927</v>
+      </c>
+      <c r="D19" t="n">
+        <v>252.7008180646225</v>
+      </c>
+      <c r="E19" t="n">
+        <v>229243.9999999999</v>
+      </c>
+      <c r="F19" t="n">
+        <v>14.92370524213183</v>
+      </c>
+      <c r="G19" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H19" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I19" t="n">
+        <v>38.0892510979685</v>
+      </c>
+      <c r="J19" t="n">
+        <v>112.5758503950789</v>
+      </c>
+      <c r="K19" t="n">
+        <v>279415.9999999999</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6034.946065878703</v>
+      </c>
+      <c r="M19" t="n">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N19" t="n">
+        <v>35.75225116085909</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P19" t="n">
+        <v>907628.9010525362</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3</v>
+      </c>
+      <c r="B20" t="n">
+        <v>5648.558240191881</v>
+      </c>
+      <c r="C20" t="n">
+        <v>27639.69999999999</v>
+      </c>
+      <c r="D20" t="n">
+        <v>271.1911218254485</v>
+      </c>
+      <c r="E20" t="n">
+        <v>794230.0365599996</v>
+      </c>
+      <c r="F20" t="n">
+        <v>32.72646118988704</v>
+      </c>
+      <c r="G20" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H20" t="n">
+        <v>125.9999999999992</v>
+      </c>
+      <c r="I20" t="n">
+        <v>95.99999999999956</v>
+      </c>
+      <c r="J20" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K20" t="n">
+        <v>378688.0000000001</v>
+      </c>
+      <c r="L20" t="n">
+        <v>11114.29774860974</v>
+      </c>
+      <c r="M20" t="n">
+        <v>8906174.164799998</v>
+      </c>
+      <c r="N20" t="n">
+        <v>35.75225116085909</v>
+      </c>
+      <c r="O20" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P20" t="n">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>3</v>
+      </c>
+      <c r="B21" t="n">
+        <v>5652.728204922643</v>
+      </c>
+      <c r="C21" t="n">
+        <v>10184.16973173145</v>
+      </c>
+      <c r="D21" t="n">
+        <v>424.9787381498739</v>
+      </c>
+      <c r="E21" t="n">
+        <v>135007.8668699999</v>
+      </c>
+      <c r="F21" t="n">
+        <v>6.047410455720619</v>
+      </c>
+      <c r="G21" t="n">
+        <v>27.9654227272727</v>
+      </c>
+      <c r="H21" t="n">
+        <v>126.9999999999992</v>
+      </c>
+      <c r="I21" t="n">
+        <v>28.66530227584867</v>
+      </c>
+      <c r="J21" t="n">
+        <v>515.0943407417118</v>
+      </c>
+      <c r="K21" t="n">
+        <v>532404</v>
+      </c>
+      <c r="L21" t="n">
+        <v>37819.7689054316</v>
+      </c>
+      <c r="M21" t="n">
+        <v>9174521.009299997</v>
+      </c>
+      <c r="N21" t="n">
+        <v>29.99999999999992</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2915.76176821649</v>
+      </c>
+      <c r="P21" t="n">
+        <v>25333054.93499543</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>5</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B22" t="n">
+        <v>3592.163814220368</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D22" t="n">
+        <v>19721.96170086985</v>
+      </c>
+      <c r="E22" t="n">
+        <v>424.6616484994997</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1094086.860592877</v>
+      </c>
+      <c r="G22" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H22" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I22" t="n">
+        <v>77.80585983126005</v>
+      </c>
+      <c r="J22" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K22" t="n">
+        <v>44036.37111627778</v>
+      </c>
+      <c r="L22" t="n">
+        <v>11411.26707998794</v>
+      </c>
+      <c r="M22" t="n">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N22" t="n">
+        <v>35.75225116085909</v>
+      </c>
+      <c r="O22" t="n">
+        <v>856.7038935390278</v>
+      </c>
+      <c r="P22" t="n">
+        <v>1248365.758196321</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>5</v>
+      </c>
+      <c r="B23" t="n">
+        <v>21239</v>
+      </c>
+      <c r="C23" t="n">
+        <v>29031.0083701363</v>
+      </c>
+      <c r="D23" t="n">
+        <v>64664.39999999999</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2077</v>
+      </c>
+      <c r="F23" t="n">
+        <v>4676977.19118</v>
+      </c>
+      <c r="G23" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="H23" t="n">
+        <v>300.9999999999981</v>
+      </c>
+      <c r="I23" t="n">
+        <v>303.9999999999987</v>
+      </c>
+      <c r="J23" t="n">
+        <v>783.7999999999988</v>
+      </c>
+      <c r="K23" t="n">
+        <v>202571</v>
+      </c>
+      <c r="L23" t="n">
+        <v>87368.90999999997</v>
+      </c>
+      <c r="M23" t="n">
+        <v>8408723.879599998</v>
+      </c>
+      <c r="N23" t="n">
+        <v>34.9999999999999</v>
+      </c>
+      <c r="O23" t="n">
+        <v>4502</v>
+      </c>
+      <c r="P23" t="n">
+        <v>25333054.93499543</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>5</v>
+      </c>
+      <c r="B24" t="n">
+        <v>15029</v>
+      </c>
+      <c r="C24" t="n">
+        <v>25869.38778</v>
+      </c>
+      <c r="D24" t="n">
+        <v>19151.02604309839</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1645.641044300649</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1067319.071699882</v>
+      </c>
+      <c r="G24" t="n">
+        <v>27.6202945590994</v>
+      </c>
+      <c r="H24" t="n">
+        <v>124.9999999999992</v>
+      </c>
+      <c r="I24" t="n">
+        <v>194.9999999999991</v>
+      </c>
+      <c r="J24" t="n">
+        <v>384.7889277610419</v>
+      </c>
+      <c r="K24" t="n">
+        <v>2168.999999999995</v>
+      </c>
+      <c r="L24" t="n">
+        <v>24766.25131576219</v>
+      </c>
+      <c r="M24" t="n">
+        <v>282905.7514288604</v>
+      </c>
+      <c r="N24" t="n">
+        <v>21.09561578308453</v>
+      </c>
+      <c r="O24" t="n">
+        <v>3211</v>
+      </c>
+      <c r="P24" t="n">
+        <v>9430951.714799995</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>5</v>
+      </c>
+      <c r="B25" t="n">
+        <v>9192</v>
+      </c>
+      <c r="C25" t="n">
+        <v>21205.02672</v>
+      </c>
+      <c r="D25" t="n">
+        <v>59994</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1042.999999999999</v>
+      </c>
+      <c r="F25" t="n">
+        <v>1194600.348719999</v>
+      </c>
+      <c r="G25" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H25" t="n">
+        <v>140.9999999999991</v>
+      </c>
+      <c r="I25" t="n">
+        <v>92.99999999999956</v>
+      </c>
+      <c r="J25" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K25" t="n">
+        <v>39877.13364253051</v>
+      </c>
+      <c r="L25" t="n">
+        <v>70633.64091748245</v>
+      </c>
+      <c r="M25" t="n">
+        <v>8271274.176000002</v>
+      </c>
+      <c r="N25" t="n">
+        <v>36.99999999999991</v>
+      </c>
+      <c r="O25" t="n">
+        <v>3090</v>
+      </c>
+      <c r="P25" t="n">
+        <v>7029925.234559999</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" t="n">
         <v>11442</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C26" t="n">
         <v>24430.4175921144</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D26" t="n">
         <v>69421.59999999999</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E26" t="n">
         <v>96.75042719463211</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F26" t="n">
         <v>3389505.0557</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G26" t="n">
         <v>27.6202945590994</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H26" t="n">
         <v>164.9999999999989</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I26" t="n">
         <v>248.999999999999</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J26" t="n">
         <v>384.7889277610419</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K26" t="n">
         <v>28977.99857868786</v>
       </c>
-      <c r="L16" t="n">
+      <c r="L26" t="n">
         <v>57789.99999999995</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M26" t="n">
         <v>827690.0633385038</v>
       </c>
-      <c r="N16" t="n">
+      <c r="N26" t="n">
         <v>5.999999999999963</v>
       </c>
-      <c r="O16" t="n">
+      <c r="O26" t="n">
         <v>3403</v>
       </c>
-      <c r="P16" t="n">
+      <c r="P26" t="n">
         <v>8379778.190979367</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>5</v>
+      </c>
+      <c r="B27" t="n">
+        <v>3245.685602352303</v>
+      </c>
+      <c r="C27" t="n">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D27" t="n">
+        <v>19721.96170086985</v>
+      </c>
+      <c r="E27" t="n">
+        <v>881.0076688693483</v>
+      </c>
+      <c r="F27" t="n">
+        <v>653758.6526362819</v>
+      </c>
+      <c r="G27" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H27" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I27" t="n">
+        <v>40.54662213654714</v>
+      </c>
+      <c r="J27" t="n">
+        <v>303.4752640467751</v>
+      </c>
+      <c r="K27" t="n">
+        <v>16059.27802363551</v>
+      </c>
+      <c r="L27" t="n">
+        <v>43983.13042192746</v>
+      </c>
+      <c r="M27" t="n">
+        <v>1887136.870938311</v>
+      </c>
+      <c r="N27" t="n">
+        <v>35.75225116085909</v>
+      </c>
+      <c r="O27" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P27" t="n">
+        <v>1405933.835730277</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>5</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2969.26732303109</v>
+      </c>
+      <c r="C28" t="n">
+        <v>22823.19152</v>
+      </c>
+      <c r="D28" t="n">
+        <v>8278.108993721817</v>
+      </c>
+      <c r="E28" t="n">
+        <v>299.833152398782</v>
+      </c>
+      <c r="F28" t="n">
+        <v>341503.8856092016</v>
+      </c>
+      <c r="G28" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H28" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I28" t="n">
+        <v>9.829484154314446</v>
+      </c>
+      <c r="J28" t="n">
+        <v>92.82369814523241</v>
+      </c>
+      <c r="K28" t="n">
+        <v>101102.9756497258</v>
+      </c>
+      <c r="L28" t="n">
+        <v>19534.24812909449</v>
+      </c>
+      <c r="M28" t="n">
+        <v>2462949.616204246</v>
+      </c>
+      <c r="N28" t="n">
+        <v>16.36044902140724</v>
+      </c>
+      <c r="O28" t="n">
+        <v>839.4548218570339</v>
+      </c>
+      <c r="P28" t="n">
+        <v>2202359.325576442</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>5</v>
+      </c>
+      <c r="B29" t="n">
+        <v>6011.999999999998</v>
+      </c>
+      <c r="C29" t="n">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D29" t="n">
+        <v>20455.99999999999</v>
+      </c>
+      <c r="E29" t="n">
+        <v>881.0076688693483</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1094086.860592877</v>
+      </c>
+      <c r="G29" t="n">
+        <v>37.19</v>
+      </c>
+      <c r="H29" t="n">
+        <v>147.9999999999991</v>
+      </c>
+      <c r="I29" t="n">
+        <v>77.80585983126005</v>
+      </c>
+      <c r="J29" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K29" t="n">
+        <v>30021.16279127876</v>
+      </c>
+      <c r="L29" t="n">
+        <v>32411.80128276228</v>
+      </c>
+      <c r="M29" t="n">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N29" t="n">
+        <v>35.75225116085909</v>
+      </c>
+      <c r="O29" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P29" t="n">
+        <v>6067714.946849998</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>5</v>
+      </c>
+      <c r="B30" t="n">
+        <v>5648.558240191881</v>
+      </c>
+      <c r="C30" t="n">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D30" t="n">
+        <v>19721.96170086985</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1097.999999999999</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1094086.860592877</v>
+      </c>
+      <c r="G30" t="n">
+        <v>51.2</v>
+      </c>
+      <c r="H30" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I30" t="n">
+        <v>45.46136421370437</v>
+      </c>
+      <c r="J30" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K30" t="n">
+        <v>43145.42334545907</v>
+      </c>
+      <c r="L30" t="n">
+        <v>32808.74048806977</v>
+      </c>
+      <c r="M30" t="n">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N30" t="n">
+        <v>17.38297708524519</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P30" t="n">
+        <v>838720.6650102267</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>5</v>
+      </c>
+      <c r="B31" t="n">
+        <v>5648.558240191881</v>
+      </c>
+      <c r="C31" t="n">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D31" t="n">
+        <v>19721.96170086985</v>
+      </c>
+      <c r="E31" t="n">
+        <v>881.0076688693483</v>
+      </c>
+      <c r="F31" t="n">
+        <v>452394.4963607445</v>
+      </c>
+      <c r="G31" t="n">
+        <v>30.8316326530612</v>
+      </c>
+      <c r="H31" t="n">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I31" t="n">
+        <v>113.9999999999995</v>
+      </c>
+      <c r="J31" t="n">
+        <v>657.7753259148542</v>
+      </c>
+      <c r="K31" t="n">
+        <v>116218</v>
+      </c>
+      <c r="L31" t="n">
+        <v>36514.42524502605</v>
+      </c>
+      <c r="M31" t="n">
+        <v>5228156.335899999</v>
+      </c>
+      <c r="N31" t="n">
+        <v>38.99999999999991</v>
+      </c>
+      <c r="O31" t="n">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P31" t="n">
+        <v>5013077.512856801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>